<commit_message>
MAINT: Corrected VaR calculation and improved unittests
</commit_message>
<xml_diff>
--- a/tests/VaR-cal.xlsx
+++ b/tests/VaR-cal.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>returns</t>
   </si>
@@ -43,14 +44,34 @@
   </si>
   <si>
     <t>Min Return with 95% prob</t>
+  </si>
+  <si>
+    <t>1 Day-Values</t>
+  </si>
+  <si>
+    <t>5 Day-Values</t>
+  </si>
+  <si>
+    <t>10 Day-Values</t>
+  </si>
+  <si>
+    <t>See documentation in gg/powerline/doc/n_day_var.ipynb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -381,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,62 +487,195 @@
         <v>0.65888433843017657</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <f>_xlfn.NORM.INV(1-D2, B9, B10)</f>
-        <v>-1.2585084656601329</v>
-      </c>
-    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <f>C2*(B11+1)</f>
-        <v>-2.1957709073171685</v>
+      <c r="A12" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <f>C2-B12</f>
-        <v>10.689770907317168</v>
+        <f>_xlfn.NORM.INV(1-D$2, B$9, B$10)</f>
+        <v>-1.2585084656601329</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <f>_xlfn.NORM.INV(1-D3, B9, B10)</f>
-        <v>-0.80948257952268254</v>
+        <f>C$2*(B13+1)</f>
+        <v>-2.1957709073171685</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <f>C2*(B14+1)</f>
-        <v>1.6182549695343345</v>
+        <f>C$2-B14</f>
+        <v>10.689770907317168</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <f>_xlfn.NORM.INV(1-D$3, B$9, B$10)</f>
+        <v>-0.80948257952268254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f>C$2*(B16+1)</f>
+        <v>1.6182549695343345</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B16">
-        <f>C2-B15</f>
+      <c r="B18">
+        <f>C$2-B17</f>
         <v>6.8757450304656658</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <f>_xlfn.NORM.INV(1-D$2, B20*B$9, SQRT(B20)*B$10)</f>
+        <v>-2.0560034104463876</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <f>C$2*(B21+1)</f>
+        <v>-8.969692968331616</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <f>C$2-B22</f>
+        <v>17.463692968331614</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <f>_xlfn.NORM.INV(1-D$3, B20*B$9, SQRT(B20)*B$10)</f>
+        <v>-1.0519510053859682</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <f>C$2*(B24+1)</f>
+        <v>-0.44127183974841383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <f>C$2-B25</f>
+        <v>8.9352718397484132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <f>_xlfn.NORM.INV(1-D$2, B28*B$9, SQRT(B28)*B$10)</f>
+        <v>-2.1042636500217209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <f>C$2*(B29+1)</f>
+        <v>-9.3796154432844965</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <f>C$2-B30</f>
+        <v>17.873615443284496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <f>_xlfn.NORM.INV(1-D$3, B28*B$9, SQRT(B28)*B$10)</f>
+        <v>-0.68431912145195151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <f>C$2*(B32+1)</f>
+        <v>2.6813933823871237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <f>C$2-B33</f>
+        <v>5.8126066176128761</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -528,7 +683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -546,4 +703,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>